<commit_message>
fix tests with excel document
</commit_message>
<xml_diff>
--- a/Examples/Resources/SampleFiles/Documents/document.xlsx
+++ b/Examples/Resources/SampleFiles/Documents/document.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Repo\Watermark\GroupDocs.Watermark-for-.NET\Examples\Resources\SampleFiles\Documents\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D029D34A-AFF8-4021-8981-0EAAEDBE625E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="15150" windowHeight="7740"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Step 1. Describe Test System" sheetId="1" r:id="rId1"/>
@@ -123,7 +129,20 @@
     <definedName name="UpFrontCostBuild">'Detailed Calculations'!$C$24</definedName>
     <definedName name="UpFrontCostBuy">'Detailed Calculations'!$C$25</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -814,11 +833,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1038,8 +1057,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="49">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1069,9 +1087,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -1090,10 +1105,9 @@
     <xf numFmtId="10" fontId="1" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -1106,8 +1120,8 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1131,7 +1145,10 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1179,13 +1196,694 @@
       <color rgb="FFE6EFF6"/>
     </mruColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
-  <c:style val="26"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'Step 1. Describe Test System'!$A$21:$A$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B83C-4838-8900-B547C0B582BD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'Step 1. Describe Test System'!$B$21:$B$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-BA71-45B2-B6E1-BD9A5DF6D864}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1423850911"/>
+        <c:axId val="1423851327"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1423850911"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1423851327"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1423851327"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1423850911"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ru-RU"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'Step 2. Verify Assumptions'!$E$17:$E$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-02B3-4E45-81A0-419C0B5BE71F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'Step 2. Verify Assumptions'!$F$17:$F$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E871-4AF0-AB1F-F793D2204565}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1423850911"/>
+        <c:axId val="1423851327"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1423850911"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1423851327"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1423851327"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1423850911"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ru-RU"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="126"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="26"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -1203,12 +1901,14 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
+      <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:areaChart>
         <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -1296,7 +1996,20 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-7140-48FB-8515-FF3987D0A61B}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:axId val="67502080"/>
         <c:axId val="98648448"/>
       </c:areaChart>
@@ -1305,6 +2018,7 @@
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -1322,24 +2036,30 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="98648448"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
         <c:axId val="98648448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="&quot;$&quot;#,##0" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="67502080"/>
         <c:crosses val="autoZero"/>
@@ -1348,9 +2068,11 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -1360,7 +2082,1463 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>4572000</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BF90F1AD-2C9B-420A-B8B2-4B4952FFDB12}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>314325</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{519F31C6-DC32-4E09-888A-2072216F3631}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8239125" y="1933575"/>
+          <a:ext cx="2286000" cy="314325"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr wrap="none" fromWordArt="1">
+          <a:prstTxWarp prst="textPlain">
+            <a:avLst/>
+          </a:prstTxWarp>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr sz="4200" kern="10" spc="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:srgbClr val="000000">
+                  <a:alpha val="100000"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:latin typeface="Times New Roman"/>
+              <a:cs typeface="Times New Roman"/>
+            </a:rPr>
+            <a:t>Test watermark</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>314325</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6E904C4E-A86B-4CD3-83D0-F36373558AF2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8239125" y="3019425"/>
+          <a:ext cx="2286000" cy="314325"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr wrap="none" fromWordArt="1">
+          <a:prstTxWarp prst="textPlain">
+            <a:avLst/>
+          </a:prstTxWarp>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="4200" kern="10" spc="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:srgbClr val="000000">
+                  <a:alpha val="100000"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:latin typeface="Times New Roman"/>
+              <a:cs typeface="Times New Roman"/>
+            </a:rPr>
+            <a:t>Shape</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="4200" kern="10" spc="0" baseline="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:srgbClr val="000000">
+                  <a:alpha val="100000"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:latin typeface="Times New Roman"/>
+              <a:cs typeface="Times New Roman"/>
+            </a:rPr>
+            <a:t> test</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>4572000</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8B7FEEDA-B9E5-487F-B9D8-65D8A2562E86}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4CA941B9-544C-4C81-89EE-2B67FF81F90A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8639175" y="1590675"/>
+          <a:ext cx="2286000" cy="314325"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr wrap="none" fromWordArt="1">
+          <a:prstTxWarp prst="textPlain">
+            <a:avLst/>
+          </a:prstTxWarp>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr sz="4200" kern="10" spc="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:srgbClr val="000000">
+                  <a:alpha val="100000"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:latin typeface="Times New Roman"/>
+              <a:cs typeface="Times New Roman"/>
+            </a:rPr>
+            <a:t>Test watermark</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>314325</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D3127EA2-0672-4E4C-B5AB-302E49E733CD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8639175" y="3105150"/>
+          <a:ext cx="2286000" cy="314325"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr wrap="none" fromWordArt="1">
+          <a:prstTxWarp prst="textPlain">
+            <a:avLst/>
+          </a:prstTxWarp>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="4200" kern="10" spc="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:srgbClr val="000000">
+                  <a:alpha val="100000"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:latin typeface="Times New Roman"/>
+              <a:cs typeface="Times New Roman"/>
+            </a:rPr>
+            <a:t>Shape</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="4200" kern="10" spc="0" baseline="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:srgbClr val="000000">
+                  <a:alpha val="100000"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:latin typeface="Times New Roman"/>
+              <a:cs typeface="Times New Roman"/>
+            </a:rPr>
+            <a:t> test</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -1377,7 +3555,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1396,9 +3580,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1436,7 +3620,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -1470,6 +3654,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1504,9 +3689,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1679,118 +3865,191 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="109.28515625" customWidth="1"/>
     <col min="2" max="2" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" ht="27.75">
-      <c r="A1" s="39" t="s">
+    <row r="1" spans="1:2" ht="27.75" x14ac:dyDescent="0.4">
+      <c r="A1" s="37" t="s">
         <v>104</v>
       </c>
-      <c r="B1" s="39"/>
-    </row>
-    <row r="2" spans="1:2" s="1" customFormat="1"/>
-    <row r="3" spans="1:2" s="1" customFormat="1" ht="21">
-      <c r="A3" s="38" t="s">
+      <c r="B1" s="37"/>
+    </row>
+    <row r="3" spans="1:2" ht="21" x14ac:dyDescent="0.25">
+      <c r="A3" s="36" t="s">
         <v>140</v>
       </c>
-      <c r="B3" s="38"/>
-    </row>
-    <row r="4" spans="1:2" s="22" customFormat="1" ht="15.75">
-      <c r="A4" s="21"/>
-      <c r="B4" s="21"/>
-    </row>
-    <row r="5" spans="1:2" ht="15.75">
-      <c r="A5" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="6" t="s">
+      <c r="B3" s="36"/>
+    </row>
+    <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="19"/>
+      <c r="B4" s="19"/>
+    </row>
+    <row r="5" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="28.5">
-      <c r="A6" s="4" t="s">
+    <row r="6" spans="1:2" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="B6" s="5"/>
-    </row>
-    <row r="7" spans="1:2" ht="28.5">
-      <c r="A7" s="4" t="s">
+      <c r="B6" s="4"/>
+    </row>
+    <row r="7" spans="1:2" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="B7" s="5"/>
-    </row>
-    <row r="8" spans="1:2" ht="28.5">
-      <c r="A8" s="4" t="s">
+      <c r="B7" s="4"/>
+    </row>
+    <row r="8" spans="1:2" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="B8" s="5"/>
-    </row>
-    <row r="9" spans="1:2" ht="28.5">
-      <c r="A9" s="4" t="s">
+      <c r="B8" s="4"/>
+    </row>
+    <row r="9" spans="1:2" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="B9" s="5"/>
-    </row>
-    <row r="10" spans="1:2" ht="28.5">
-      <c r="A10" s="4" t="s">
+      <c r="B9" s="4"/>
+    </row>
+    <row r="10" spans="1:2" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="B10" s="5"/>
-    </row>
-    <row r="11" spans="1:2" ht="41.25">
-      <c r="A11" s="4" t="s">
+      <c r="B10" s="4"/>
+    </row>
+    <row r="11" spans="1:2" ht="41.25" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="B11" s="5"/>
-    </row>
-    <row r="12" spans="1:2" ht="28.5">
-      <c r="A12" s="4" t="s">
+      <c r="B11" s="4"/>
+    </row>
+    <row r="12" spans="1:2" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="B12" s="5"/>
-    </row>
-    <row r="13" spans="1:2" ht="28.5">
-      <c r="A13" s="4" t="s">
+      <c r="B12" s="4"/>
+    </row>
+    <row r="13" spans="1:2" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="B13" s="5"/>
-    </row>
-    <row r="14" spans="1:2" ht="28.5">
-      <c r="A14" s="4" t="s">
+      <c r="B13" s="4"/>
+    </row>
+    <row r="14" spans="1:2" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="B14" s="5"/>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="B16" s="7" t="s">
+      <c r="B14" s="4"/>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B16" s="6" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
-      <c r="B17" s="8" t="s">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B17" s="7" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
-      <c r="B18" s="8" t="s">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B18" s="7" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
-      <c r="A19" s="1"/>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" s="1"/>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>1</v>
+      </c>
+      <c r="B21">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>2</v>
+      </c>
+      <c r="B22">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>3</v>
+      </c>
+      <c r="B23">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>4</v>
+      </c>
+      <c r="B24">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>5</v>
+      </c>
+      <c r="B25">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>6</v>
+      </c>
+      <c r="B26">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>7</v>
+      </c>
+      <c r="B27">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>8</v>
+      </c>
+      <c r="B28">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>9</v>
+      </c>
+      <c r="B29">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>10</v>
+      </c>
+      <c r="B30">
+        <v>1000</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1798,536 +4057,596 @@
     <mergeCell ref="A1:B1"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="decimal" operator="greaterThan" showInputMessage="1" showErrorMessage="1" sqref="B6:B14">
+    <dataValidation type="decimal" operator="greaterThan" showInputMessage="1" showErrorMessage="1" sqref="B6:B14" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>0</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="B17" location="'Step 2. Verify Assumptions'!A1" display="View and verify assumptions"/>
-    <hyperlink ref="B18" location="'Step 3. Results'!A1" display="Go directly to results"/>
+    <hyperlink ref="B17" location="'Step 2. Verify Assumptions'!A1" display="View and verify assumptions" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B18" location="'Step 3. Results'!A1" display="Go directly to results" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E51"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:F51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.7109375" style="10" customWidth="1"/>
-    <col min="2" max="2" width="110.5703125" style="10" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" style="10" customWidth="1"/>
-    <col min="4" max="5" width="14.28515625" style="10" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="10"/>
+    <col min="1" max="1" width="3.7109375" style="9" customWidth="1"/>
+    <col min="2" max="2" width="110.5703125" style="9" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" style="9" customWidth="1"/>
+    <col min="4" max="5" width="14.28515625" style="9" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" ht="27.75">
-      <c r="A1" s="39" t="s">
+    <row r="1" spans="1:5" customFormat="1" ht="27.75" x14ac:dyDescent="0.4">
+      <c r="A1" s="37" t="s">
         <v>104</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-    </row>
-    <row r="2" spans="1:5" s="1" customFormat="1"/>
-    <row r="3" spans="1:5" s="27" customFormat="1" ht="21" customHeight="1">
-      <c r="A3" s="28" t="s">
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+    </row>
+    <row r="2" spans="1:5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:5" s="24" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="25" t="s">
         <v>141</v>
       </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="29" t="s">
+      <c r="B3"/>
+      <c r="C3"/>
+      <c r="D3"/>
+      <c r="E3"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="26" t="s">
         <v>142</v>
       </c>
-      <c r="D4" s="1"/>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="D5" s="1"/>
-    </row>
-    <row r="6" spans="1:5" ht="15.75">
-      <c r="A6" s="23" t="s">
+      <c r="D4"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D5"/>
+    </row>
+    <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="20" t="s">
         <v>118</v>
       </c>
-      <c r="B6" s="24"/>
-      <c r="C6" s="24"/>
-      <c r="D6" s="1"/>
-    </row>
-    <row r="7" spans="1:5" ht="15.75">
-      <c r="A7" s="12"/>
-      <c r="B7" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="C7" s="12" t="s">
+      <c r="B6" s="21"/>
+      <c r="C6" s="21"/>
+      <c r="D6"/>
+    </row>
+    <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="11"/>
+      <c r="B7" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="1"/>
-      <c r="E7" s="11"/>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="30"/>
-      <c r="B8" s="30" t="s">
+      <c r="D7"/>
+      <c r="E7" s="10"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="27"/>
+      <c r="B8" s="27" t="s">
         <v>119</v>
       </c>
-      <c r="C8" s="5">
-        <v>0</v>
-      </c>
-      <c r="D8" s="1"/>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="30"/>
-      <c r="B9" s="30" t="s">
+      <c r="C8" s="4">
+        <v>0</v>
+      </c>
+      <c r="D8"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="27"/>
+      <c r="B9" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="4">
         <f>AvgSalaryDeveloper</f>
         <v>0</v>
       </c>
-      <c r="D9" s="1"/>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="30"/>
-      <c r="B10" s="30" t="s">
+      <c r="D9" s="35"/>
+      <c r="E9"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="27"/>
+      <c r="B10" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="4">
         <v>250</v>
       </c>
-      <c r="D10" s="1"/>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="D11" s="1"/>
-    </row>
-    <row r="12" spans="1:5" ht="15.75">
-      <c r="A12" s="23" t="s">
+      <c r="D10"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D11"/>
+    </row>
+    <row r="12" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="20" t="s">
         <v>120</v>
       </c>
-      <c r="B12" s="24"/>
-      <c r="C12" s="24"/>
-      <c r="D12" s="1"/>
-    </row>
-    <row r="13" spans="1:5" ht="15.75">
-      <c r="A13" s="12"/>
-      <c r="B13" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="C13" s="12" t="s">
+      <c r="B12" s="21"/>
+      <c r="C12" s="21"/>
+      <c r="D12"/>
+    </row>
+    <row r="13" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="11"/>
+      <c r="B13" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="D13" s="1"/>
-      <c r="E13" s="11"/>
-    </row>
-    <row r="14" spans="1:5" ht="27.75">
-      <c r="A14" s="32"/>
-      <c r="B14" s="32" t="s">
+      <c r="D13"/>
+      <c r="E13" s="10"/>
+    </row>
+    <row r="14" spans="1:5" ht="27.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="29"/>
+      <c r="B14" s="29" t="s">
         <v>124</v>
       </c>
-      <c r="C14" s="5">
+      <c r="C14" s="4">
         <v>20</v>
       </c>
-      <c r="D14" s="1"/>
-    </row>
-    <row r="15" spans="1:5" ht="27.75">
-      <c r="A15" s="32"/>
-      <c r="B15" s="32" t="s">
+      <c r="D14"/>
+    </row>
+    <row r="15" spans="1:5" ht="27.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="29"/>
+      <c r="B15" s="29" t="s">
         <v>125</v>
       </c>
-      <c r="C15" s="5">
+      <c r="C15" s="4">
         <v>40</v>
       </c>
-      <c r="D15" s="1"/>
-    </row>
-    <row r="16" spans="1:5" ht="27.75">
-      <c r="A16" s="32"/>
-      <c r="B16" s="32" t="s">
+      <c r="D15"/>
+    </row>
+    <row r="16" spans="1:5" ht="27.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="29"/>
+      <c r="B16" s="29" t="s">
         <v>126</v>
       </c>
-      <c r="C16" s="5">
+      <c r="C16" s="4">
         <v>40</v>
       </c>
-      <c r="D16" s="1"/>
-    </row>
-    <row r="17" spans="1:5" ht="27.75">
-      <c r="A17" s="32"/>
-      <c r="B17" s="32" t="s">
+      <c r="D16"/>
+    </row>
+    <row r="17" spans="1:6" ht="27.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="29"/>
+      <c r="B17" s="29" t="s">
         <v>128</v>
       </c>
-      <c r="C17" s="5">
+      <c r="C17" s="4">
         <v>5</v>
       </c>
-      <c r="D17" s="1"/>
-    </row>
-    <row r="18" spans="1:5" ht="27.75" customHeight="1">
-      <c r="A18" s="32"/>
-      <c r="B18" s="32" t="s">
+      <c r="D17"/>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="29"/>
+      <c r="B18" s="29" t="s">
         <v>127</v>
       </c>
-      <c r="C18" s="5">
+      <c r="C18" s="4">
         <v>25000</v>
       </c>
-      <c r="D18" s="1"/>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="B19" s="11"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="11"/>
-    </row>
-    <row r="20" spans="1:5" ht="15.75">
-      <c r="A20" s="23" t="s">
+      <c r="D18"/>
+      <c r="E18">
+        <v>2</v>
+      </c>
+      <c r="F18">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B19" s="10"/>
+      <c r="C19" s="10"/>
+      <c r="D19"/>
+      <c r="E19">
+        <v>3</v>
+      </c>
+      <c r="F19">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="20" t="s">
         <v>121</v>
       </c>
-      <c r="B20" s="24"/>
-      <c r="C20" s="24"/>
-      <c r="D20" s="1"/>
-    </row>
-    <row r="21" spans="1:5" ht="15.75">
-      <c r="A21" s="12"/>
-      <c r="B21" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="C21" s="12" t="s">
+      <c r="B20" s="21"/>
+      <c r="C20" s="21"/>
+      <c r="D20"/>
+      <c r="E20">
+        <v>4</v>
+      </c>
+      <c r="F20">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="11"/>
+      <c r="B21" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C21" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="D21" s="1"/>
-      <c r="E21" s="11"/>
-    </row>
-    <row r="22" spans="1:5" ht="27.75">
-      <c r="A22" s="32"/>
-      <c r="B22" s="32" t="s">
+      <c r="D21"/>
+      <c r="E21">
+        <v>5</v>
+      </c>
+      <c r="F21">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="27.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="29"/>
+      <c r="B22" s="29" t="s">
         <v>129</v>
       </c>
-      <c r="C22" s="5">
+      <c r="C22" s="4">
         <v>5</v>
       </c>
-      <c r="D22" s="1"/>
-    </row>
-    <row r="23" spans="1:5" ht="27.75">
-      <c r="A23" s="32"/>
-      <c r="B23" s="32" t="s">
+      <c r="D22"/>
+      <c r="E22">
+        <v>6</v>
+      </c>
+      <c r="F22">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="27.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="29"/>
+      <c r="B23" s="29" t="s">
         <v>130</v>
       </c>
-      <c r="C23" s="5">
+      <c r="C23" s="4">
         <v>15</v>
       </c>
-      <c r="D23" s="1"/>
-    </row>
-    <row r="24" spans="1:5" ht="27.75">
-      <c r="A24" s="32"/>
-      <c r="B24" s="32" t="s">
+      <c r="D23"/>
+      <c r="E23">
+        <v>7</v>
+      </c>
+      <c r="F23">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="27.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="29"/>
+      <c r="B24" s="29" t="s">
         <v>131</v>
       </c>
-      <c r="C24" s="5">
+      <c r="C24" s="4">
         <v>5</v>
       </c>
-      <c r="D24" s="1"/>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="D25" s="1"/>
-    </row>
-    <row r="26" spans="1:5" ht="15.75">
-      <c r="A26" s="25" t="s">
+      <c r="D24"/>
+      <c r="E24">
+        <v>8</v>
+      </c>
+      <c r="F24">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D25"/>
+      <c r="E25">
+        <v>9</v>
+      </c>
+      <c r="F25">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="22" t="s">
         <v>122</v>
       </c>
-      <c r="B26" s="26"/>
-      <c r="C26" s="26"/>
-      <c r="D26" s="1"/>
-    </row>
-    <row r="27" spans="1:5" ht="15.75">
-      <c r="A27" s="12"/>
-      <c r="B27" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="C27" s="12" t="s">
+      <c r="B26" s="23"/>
+      <c r="C26" s="23"/>
+      <c r="D26"/>
+      <c r="E26">
+        <v>10</v>
+      </c>
+      <c r="F26">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="11"/>
+      <c r="B27" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C27" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="D27" s="1"/>
-      <c r="E27" s="11"/>
-    </row>
-    <row r="28" spans="1:5">
-      <c r="A28" s="32"/>
-      <c r="B28" s="30" t="s">
+      <c r="D27"/>
+      <c r="E27" s="10"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="29"/>
+      <c r="B28" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="C28" s="5">
+      <c r="C28" s="4">
         <v>3899</v>
       </c>
-      <c r="D28" s="1"/>
-    </row>
-    <row r="29" spans="1:5">
-      <c r="A29" s="32"/>
-      <c r="B29" s="30" t="s">
+      <c r="D28"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="29"/>
+      <c r="B29" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="C29" s="5">
+      <c r="C29" s="4">
         <v>529</v>
       </c>
-      <c r="D29" s="1"/>
-    </row>
-    <row r="30" spans="1:5">
-      <c r="A30" s="32"/>
-      <c r="B30" s="30" t="s">
+      <c r="D29"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="29"/>
+      <c r="B30" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="C30" s="5">
+      <c r="C30" s="4">
         <v>779</v>
       </c>
-      <c r="D30" s="1"/>
-    </row>
-    <row r="31" spans="1:5">
-      <c r="A31" s="32"/>
-      <c r="B31" s="30" t="s">
+      <c r="D30"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="29"/>
+      <c r="B31" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="C31" s="5">
+      <c r="C31" s="4">
         <v>2100</v>
       </c>
-      <c r="D31" s="1"/>
-    </row>
-    <row r="33" spans="1:5" ht="15.75">
-      <c r="A33" s="45" t="s">
+      <c r="D31"/>
+    </row>
+    <row r="33" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A33" s="43" t="s">
         <v>123</v>
       </c>
-      <c r="B33" s="46"/>
-      <c r="C33" s="46"/>
-      <c r="D33" s="46"/>
-      <c r="E33" s="47"/>
-    </row>
-    <row r="34" spans="1:5" ht="15.75">
-      <c r="A34" s="40"/>
-      <c r="B34" s="43" t="s">
+      <c r="B33" s="44"/>
+      <c r="C33" s="44"/>
+      <c r="D33" s="44"/>
+      <c r="E33" s="45"/>
+    </row>
+    <row r="34" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="38"/>
+      <c r="B34" s="41" t="s">
         <v>132</v>
       </c>
-      <c r="C34" s="41" t="s">
+      <c r="C34" s="39" t="s">
         <v>136</v>
       </c>
-      <c r="D34" s="40" t="s">
+      <c r="D34" s="38" t="s">
         <v>135</v>
       </c>
-      <c r="E34" s="40"/>
-    </row>
-    <row r="35" spans="1:5" ht="15.75">
-      <c r="A35" s="40"/>
-      <c r="B35" s="44"/>
-      <c r="C35" s="42"/>
-      <c r="D35" s="13" t="s">
+      <c r="E34" s="38"/>
+    </row>
+    <row r="35" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A35" s="38"/>
+      <c r="B35" s="42"/>
+      <c r="C35" s="40"/>
+      <c r="D35" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="E35" s="13" t="s">
+      <c r="E35" s="12" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="36" spans="1:5">
-      <c r="A36" s="30"/>
-      <c r="B36" s="30" t="s">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="27"/>
+      <c r="B36" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="C36" s="5">
+      <c r="C36" s="4">
         <v>1</v>
       </c>
-      <c r="D36" s="15">
+      <c r="D36" s="13">
         <v>100</v>
       </c>
-      <c r="E36" s="15">
+      <c r="E36" s="13">
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:5">
-      <c r="A37" s="30"/>
-      <c r="B37" s="30" t="s">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="27"/>
+      <c r="B37" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="C37" s="5">
+      <c r="C37" s="4">
         <v>1</v>
       </c>
-      <c r="D37" s="15">
+      <c r="D37" s="13">
         <v>40</v>
       </c>
-      <c r="E37" s="15">
+      <c r="E37" s="13">
         <v>8</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
-      <c r="A38" s="30"/>
-      <c r="B38" s="30" t="s">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="27"/>
+      <c r="B38" s="27" t="s">
         <v>84</v>
       </c>
-      <c r="C38" s="5">
+      <c r="C38" s="4">
         <v>1</v>
       </c>
-      <c r="D38" s="15">
+      <c r="D38" s="13">
         <v>15</v>
       </c>
-      <c r="E38" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5">
-      <c r="A39" s="30"/>
-      <c r="B39" s="30" t="s">
+      <c r="E38" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="27"/>
+      <c r="B39" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="C39" s="5">
+      <c r="C39" s="4">
         <v>1</v>
       </c>
-      <c r="D39" s="15">
+      <c r="D39" s="13">
         <v>10</v>
       </c>
-      <c r="E39" s="15">
+      <c r="E39" s="13">
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:5">
-      <c r="A40" s="30"/>
-      <c r="B40" s="30" t="s">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="27"/>
+      <c r="B40" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="C40" s="5">
+      <c r="C40" s="4">
         <v>1</v>
       </c>
-      <c r="D40" s="15">
+      <c r="D40" s="13">
         <v>15</v>
       </c>
-      <c r="E40" s="15">
+      <c r="E40" s="13">
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:5">
-      <c r="A41" s="30"/>
-      <c r="B41" s="30" t="s">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="27"/>
+      <c r="B41" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="C41" s="5">
+      <c r="C41" s="4">
         <v>1</v>
       </c>
-      <c r="D41" s="15">
+      <c r="D41" s="13">
         <v>5</v>
       </c>
-      <c r="E41" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5">
-      <c r="A42" s="30"/>
-      <c r="B42" s="30" t="s">
+      <c r="E41" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="27"/>
+      <c r="B42" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="C42" s="5">
+      <c r="C42" s="4">
         <v>1</v>
       </c>
-      <c r="D42" s="15">
+      <c r="D42" s="13">
         <v>100</v>
       </c>
-      <c r="E42" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5">
-      <c r="A43" s="30"/>
-      <c r="B43" s="30" t="s">
+      <c r="E42" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="27"/>
+      <c r="B43" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="C43" s="5">
+      <c r="C43" s="4">
         <v>1</v>
       </c>
-      <c r="D43" s="15">
+      <c r="D43" s="13">
         <v>5</v>
       </c>
-      <c r="E43" s="15">
+      <c r="E43" s="13">
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:5">
-      <c r="A44" s="30"/>
-      <c r="B44" s="30" t="s">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="27"/>
+      <c r="B44" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="C44" s="5">
+      <c r="C44" s="4">
         <v>1</v>
       </c>
-      <c r="D44" s="15">
+      <c r="D44" s="13">
         <v>15</v>
       </c>
-      <c r="E44" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5">
-      <c r="A45" s="31"/>
-      <c r="B45" s="31" t="s">
+      <c r="E44" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="28"/>
+      <c r="B45" s="28" t="s">
         <v>133</v>
       </c>
-      <c r="C45" s="9" t="s">
+      <c r="C45" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="D45" s="15">
+      <c r="D45" s="13">
         <v>5</v>
       </c>
-      <c r="E45" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5">
-      <c r="A46" s="30"/>
-      <c r="B46" s="30" t="s">
+      <c r="E45" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="27"/>
+      <c r="B46" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="C46" s="5">
+      <c r="C46" s="4">
         <v>1</v>
       </c>
-      <c r="D46" s="15">
+      <c r="D46" s="13">
         <v>20</v>
       </c>
-      <c r="E46" s="15">
+      <c r="E46" s="13">
         <v>3</v>
       </c>
     </row>
-    <row r="47" spans="1:5">
-      <c r="A47" s="30"/>
-      <c r="B47" s="30" t="s">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="27"/>
+      <c r="B47" s="27" t="s">
         <v>82</v>
       </c>
-      <c r="C47" s="5">
+      <c r="C47" s="4">
         <v>1</v>
       </c>
-      <c r="D47" s="15">
+      <c r="D47" s="13">
         <v>15</v>
       </c>
-      <c r="E47" s="15">
+      <c r="E47" s="13">
         <v>2</v>
       </c>
     </row>
-    <row r="48" spans="1:5">
-      <c r="A48" s="30"/>
-      <c r="B48" s="30" t="s">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="27"/>
+      <c r="B48" s="27" t="s">
         <v>83</v>
       </c>
-      <c r="C48" s="5">
+      <c r="C48" s="4">
         <v>1</v>
       </c>
-      <c r="D48" s="15">
+      <c r="D48" s="13">
         <v>20</v>
       </c>
-      <c r="E48" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="5:5">
-      <c r="E50" s="7" t="s">
+      <c r="E48" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E50" s="6" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="51" spans="5:5">
-      <c r="E51" s="8" t="s">
+    <row r="51" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E51" s="7" t="s">
         <v>137</v>
       </c>
     </row>
@@ -2341,427 +4660,364 @@
     <mergeCell ref="A34:A35"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="E51" location="'Step 3. Results'!A1" display="Go directly to results"/>
+    <hyperlink ref="E51" location="'Step 3. Results'!A1" display="Go directly to results" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.7109375" customWidth="1"/>
     <col min="2" max="2" width="39.42578125" customWidth="1"/>
     <col min="3" max="3" width="16.5703125" customWidth="1"/>
-    <col min="4" max="4" width="15.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="10.5703125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" ht="27.75">
-      <c r="A1" s="39" t="s">
+    <row r="1" spans="1:7" ht="27.75" x14ac:dyDescent="0.4">
+      <c r="A1" s="37" t="s">
         <v>104</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-    </row>
-    <row r="2" spans="1:7" s="1" customFormat="1">
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="3"/>
-    </row>
-    <row r="3" spans="1:7" s="1" customFormat="1" ht="21">
-      <c r="A3" s="28" t="s">
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+    </row>
+    <row r="3" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="A3" s="25" t="s">
         <v>143</v>
       </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="3"/>
-    </row>
-    <row r="4" spans="1:7" s="1" customFormat="1">
-      <c r="A4" s="36" t="str">
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="33" t="str">
         <f>"You will save " &amp;TEXT((E12), "$0,000") &amp;" (" &amp;TEXT((E12/B12), "0.0%") &amp;") by buying a COTS test executive over building your own over the first 5 years of your test system"</f>
         <v>You will save $25,000 (100.0%) by buying a COTS test executive over building your own over the first 5 years of your test system</v>
       </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="3"/>
-    </row>
-    <row r="5" spans="1:7" s="1" customFormat="1" ht="21">
-      <c r="A5" s="28"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="3"/>
-    </row>
-    <row r="6" spans="1:7" s="1" customFormat="1" ht="15.75">
-      <c r="A6" s="14" t="s">
+    </row>
+    <row r="5" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="A5" s="25"/>
+    </row>
+    <row r="6" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="D6" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="E6" s="14" t="s">
+      <c r="E6" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="F6" s="3"/>
-    </row>
-    <row r="7" spans="1:7" s="1" customFormat="1">
-      <c r="A7" s="33">
-        <v>0</v>
-      </c>
-      <c r="B7" s="37">
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="30">
+        <v>0</v>
+      </c>
+      <c r="B7" s="34">
         <f>UpFrontCostBuild</f>
         <v>25000</v>
       </c>
-      <c r="C7" s="37">
+      <c r="C7" s="34">
         <f>UpFrontCostBuy</f>
         <v>0</v>
       </c>
-      <c r="D7" s="37">
-        <v>0</v>
-      </c>
-      <c r="E7" s="37">
+      <c r="D7" s="34">
+        <v>0</v>
+      </c>
+      <c r="E7" s="34">
         <f>B7-C7</f>
         <v>25000</v>
       </c>
-      <c r="F7" s="3"/>
-    </row>
-    <row r="8" spans="1:7" s="1" customFormat="1">
-      <c r="A8" s="33">
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="30">
         <v>1</v>
       </c>
-      <c r="B8" s="37">
+      <c r="B8" s="34">
         <f>(CostMaintainTestSystemRecurringBaseBuild * ((1 + IncreaseInMaintenance_percent/100) ^ (A8-1))) + CostReviseTrainingMaterialBuild + CostTrainingEmployeesRecurringBuild +B7</f>
         <v>25000</v>
       </c>
-      <c r="C8" s="37">
+      <c r="C8" s="34">
         <f>(CostMaintainTestSystemRecurringBaseBuy * ((1 + IncreaseInMaintenance_percent/100) ^ (A8-1))) + CostReviseTrainingMaterialBuy + CostTrainingEmployeesRecurringBuy + C7</f>
         <v>0</v>
       </c>
-      <c r="D8" s="37">
-        <v>0</v>
-      </c>
-      <c r="E8" s="37">
+      <c r="D8" s="34">
+        <v>0</v>
+      </c>
+      <c r="E8" s="34">
         <f t="shared" ref="E8:E12" si="0">B8-C8</f>
         <v>25000</v>
       </c>
-      <c r="F8" s="3"/>
-    </row>
-    <row r="9" spans="1:7" s="1" customFormat="1">
-      <c r="A9" s="33">
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="30">
         <v>2</v>
       </c>
-      <c r="B9" s="37">
+      <c r="B9" s="34">
         <f>(CostMaintainTestSystemRecurringBaseBuild * ((1 + IncreaseInMaintenance_percent/100) ^ (A9-1))) + CostReviseTrainingMaterialBuild + CostTrainingEmployeesRecurringBuild +B8</f>
         <v>25000</v>
       </c>
-      <c r="C9" s="37">
+      <c r="C9" s="34">
         <f>(CostMaintainTestSystemRecurringBaseBuy * ((1 + IncreaseInMaintenance_percent/100) ^ (A9-1))) + CostReviseTrainingMaterialBuy + CostTrainingEmployeesRecurringBuy +C8</f>
         <v>0</v>
       </c>
-      <c r="D9" s="37">
-        <v>0</v>
-      </c>
-      <c r="E9" s="37">
+      <c r="D9" s="34">
+        <v>0</v>
+      </c>
+      <c r="E9" s="34">
         <f t="shared" si="0"/>
         <v>25000</v>
       </c>
-      <c r="F9" s="3"/>
-    </row>
-    <row r="10" spans="1:7" s="1" customFormat="1">
-      <c r="A10" s="33">
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="30">
         <v>3</v>
       </c>
-      <c r="B10" s="37">
+      <c r="B10" s="34">
         <f>(CostMaintainTestSystemRecurringBaseBuild * ((1 + IncreaseInMaintenance_percent/100) ^ (A10-1))) + CostReviseTrainingMaterialBuild + CostTrainingEmployeesRecurringBuild +B9</f>
         <v>25000</v>
       </c>
-      <c r="C10" s="37">
+      <c r="C10" s="34">
         <f>(CostMaintainTestSystemRecurringBaseBuy * ((1 + IncreaseInMaintenance_percent/100) ^ (A10-1))) + CostReviseTrainingMaterialBuy + CostTrainingEmployeesRecurringBuy +C9</f>
         <v>0</v>
       </c>
-      <c r="D10" s="37">
-        <v>0</v>
-      </c>
-      <c r="E10" s="37">
+      <c r="D10" s="34">
+        <v>0</v>
+      </c>
+      <c r="E10" s="34">
         <f t="shared" si="0"/>
         <v>25000</v>
       </c>
-      <c r="F10" s="3"/>
-    </row>
-    <row r="11" spans="1:7" s="1" customFormat="1">
-      <c r="A11" s="33">
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="30">
         <v>4</v>
       </c>
-      <c r="B11" s="37">
+      <c r="B11" s="34">
         <f>(CostMaintainTestSystemRecurringBaseBuild * ((1 + IncreaseInMaintenance_percent/100) ^ (A11-1))) + CostReviseTrainingMaterialBuild + CostTrainingEmployeesRecurringBuild +B10</f>
         <v>25000</v>
       </c>
-      <c r="C11" s="37">
+      <c r="C11" s="34">
         <f>(CostMaintainTestSystemRecurringBaseBuy * ((1 + IncreaseInMaintenance_percent/100) ^ (A11-1))) + CostReviseTrainingMaterialBuy + CostTrainingEmployeesRecurringBuy +C10</f>
         <v>0</v>
       </c>
-      <c r="D11" s="37">
-        <v>0</v>
-      </c>
-      <c r="E11" s="37">
+      <c r="D11" s="34">
+        <v>0</v>
+      </c>
+      <c r="E11" s="34">
         <f t="shared" si="0"/>
         <v>25000</v>
       </c>
-      <c r="F11" s="3"/>
-    </row>
-    <row r="12" spans="1:7" s="1" customFormat="1">
-      <c r="A12" s="33">
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="30">
         <v>5</v>
       </c>
-      <c r="B12" s="37">
+      <c r="B12" s="34">
         <f>(CostMaintainTestSystemRecurringBaseBuild * ((1 + IncreaseInMaintenance_percent/100) ^ (A12-1))) + CostReviseTrainingMaterialBuild + CostTrainingEmployeesRecurringBuild +B11</f>
         <v>25000</v>
       </c>
-      <c r="C12" s="37">
+      <c r="C12" s="34">
         <f>(CostMaintainTestSystemRecurringBaseBuy * ((1 + IncreaseInMaintenance_percent/100) ^ (A12-1))) + CostReviseTrainingMaterialBuy + CostTrainingEmployeesRecurringBuy +C11</f>
         <v>0</v>
       </c>
-      <c r="D12" s="37">
-        <v>0</v>
-      </c>
-      <c r="E12" s="37">
+      <c r="D12" s="34">
+        <v>0</v>
+      </c>
+      <c r="E12" s="34">
         <f t="shared" si="0"/>
         <v>25000</v>
       </c>
-      <c r="F12" s="3"/>
-    </row>
-    <row r="13" spans="1:7" s="1" customFormat="1">
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="3"/>
-    </row>
-    <row r="14" spans="1:7" s="1" customFormat="1">
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="3"/>
-    </row>
-    <row r="15" spans="1:7" s="1" customFormat="1">
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="3"/>
-    </row>
-    <row r="16" spans="1:7" s="1" customFormat="1">
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="3"/>
-    </row>
-    <row r="17" spans="1:6" s="1" customFormat="1">
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="3"/>
-    </row>
-    <row r="18" spans="1:6" s="1" customFormat="1">
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="3"/>
-    </row>
-    <row r="19" spans="1:6" s="1" customFormat="1">
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="3"/>
-    </row>
-    <row r="20" spans="1:6" s="1" customFormat="1">
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="3"/>
-    </row>
-    <row r="21" spans="1:6" s="1" customFormat="1" ht="21">
-      <c r="A21" s="28" t="s">
+    </row>
+    <row r="21" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A21" s="25" t="s">
         <v>139</v>
       </c>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="3"/>
-    </row>
-    <row r="22" spans="1:6">
-      <c r="A22" s="36" t="str">
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="33" t="str">
         <f>"You will save " &amp;TEXT((C31-D31), "$0,000") &amp;" (" &amp;TEXT(E31, "0.0%") &amp;") by buying a COTS test executive over building your own over the lifetime of your test system"</f>
         <v>You will save $25,000 (100.0%) by buying a COTS test executive over building your own over the lifetime of your test system</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="15.75">
-      <c r="A23" s="45"/>
-      <c r="B23" s="47"/>
-      <c r="C23" s="14" t="s">
+    <row r="23" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="43"/>
+      <c r="B23" s="45"/>
+      <c r="C23" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="D23" s="14" t="s">
+      <c r="D23" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="E23" s="14" t="s">
+      <c r="E23" s="11" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
-      <c r="A24" s="48" t="s">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="46" t="s">
         <v>60</v>
       </c>
-      <c r="B24" s="48"/>
-      <c r="C24" s="19">
+      <c r="B24" s="46"/>
+      <c r="C24" s="17">
         <f>C25+C26</f>
         <v>0</v>
       </c>
-      <c r="D24" s="19">
+      <c r="D24" s="17">
         <f>D25+D26</f>
         <v>0</v>
       </c>
-      <c r="E24" s="20" t="e">
+      <c r="E24" s="18" t="e">
         <f t="shared" ref="E24:E31" si="1">(C24-D24)/C24</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
-      <c r="A25" s="33"/>
-      <c r="B25" s="33" t="s">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="30"/>
+      <c r="B25" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="C25" s="34">
+      <c r="C25" s="31">
         <f>CostDevelopTestExecutiveBuild</f>
         <v>0</v>
       </c>
-      <c r="D25" s="34">
+      <c r="D25" s="31">
         <f>CostDevelopTestExecutiveBuy</f>
         <v>0</v>
       </c>
-      <c r="E25" s="35" t="e">
+      <c r="E25" s="32" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
-      <c r="A26" s="33"/>
-      <c r="B26" s="33" t="s">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="30"/>
+      <c r="B26" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="C26" s="34">
+      <c r="C26" s="31">
         <f>CostMaintainTestSystemTotalBuild</f>
         <v>0</v>
       </c>
-      <c r="D26" s="34">
+      <c r="D26" s="31">
         <f>CostMaintainTestSystemTotalBuy</f>
         <v>0</v>
       </c>
-      <c r="E26" s="35" t="e">
+      <c r="E26" s="32" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
-      <c r="A27" s="48" t="s">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="46" t="s">
         <v>59</v>
       </c>
-      <c r="B27" s="48"/>
-      <c r="C27" s="19">
+      <c r="B27" s="46"/>
+      <c r="C27" s="17">
         <f>C28+C29+C30</f>
         <v>25000</v>
       </c>
-      <c r="D27" s="19">
+      <c r="D27" s="17">
         <f>D28+D29+D30</f>
         <v>0</v>
       </c>
-      <c r="E27" s="20">
+      <c r="E27" s="18">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
-      <c r="A28" s="33"/>
-      <c r="B28" s="33" t="s">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="30"/>
+      <c r="B28" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="C28" s="34">
+      <c r="C28" s="31">
         <f>CostDevelopTrainingMaterialBuild</f>
         <v>0</v>
       </c>
-      <c r="D28" s="34">
+      <c r="D28" s="31">
         <f>CostDevelopTrainingMaterialBuy</f>
         <v>0</v>
       </c>
-      <c r="E28" s="35" t="e">
+      <c r="E28" s="32" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
-      <c r="A29" s="33"/>
-      <c r="B29" s="33" t="s">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="30"/>
+      <c r="B29" s="30" t="s">
         <v>57</v>
       </c>
-      <c r="C29" s="34">
+      <c r="C29" s="31">
         <f>CostReviseTrainingMaterialTotalBuild</f>
         <v>0</v>
       </c>
-      <c r="D29" s="34">
+      <c r="D29" s="31">
         <f>CostReviseTrainingMaterialTotalBuy</f>
         <v>0</v>
       </c>
-      <c r="E29" s="35" t="e">
+      <c r="E29" s="32" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
-      <c r="A30" s="33"/>
-      <c r="B30" s="33" t="s">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="30"/>
+      <c r="B30" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="C30" s="34">
+      <c r="C30" s="31">
         <f>CostTrainingEmployeesTotalBuild</f>
         <v>25000</v>
       </c>
-      <c r="D30" s="34">
+      <c r="D30" s="31">
         <f>CostTrainingEmployeesTotalBuy</f>
         <v>0</v>
       </c>
-      <c r="E30" s="35">
+      <c r="E30" s="32">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="15.75">
-      <c r="A31" s="42" t="s">
+    <row r="31" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A31" s="40" t="s">
         <v>58</v>
       </c>
-      <c r="B31" s="42"/>
-      <c r="C31" s="18">
+      <c r="B31" s="40"/>
+      <c r="C31" s="16">
         <f>C24+C27</f>
         <v>25000</v>
       </c>
-      <c r="D31" s="18">
+      <c r="D31" s="16">
         <f>D24+D27</f>
         <v>0</v>
       </c>
-      <c r="E31" s="17">
+      <c r="E31" s="15">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="4:4" customFormat="1" ht="21">
-      <c r="D38" s="28"/>
+    <row r="38" spans="4:4" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="D38" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -2778,454 +5034,451 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E39"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A3:C39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="44" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="147.28515625" customWidth="1"/>
     <col min="3" max="3" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1"/>
-    <row r="2" spans="1:5" s="1" customFormat="1"/>
-    <row r="3" spans="1:5" ht="15.75">
-      <c r="A3" s="12" t="s">
+    <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="11" t="s">
         <v>138</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="11" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="30" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="30" t="s">
+      <c r="B4" s="27" t="s">
         <v>91</v>
       </c>
-      <c r="C4" s="16">
+      <c r="C4" s="14">
         <f>TimeToDevelopTestSystemBuild * CostPerDayDeveloper</f>
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="30" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="30" t="s">
+      <c r="B5" s="27" t="s">
         <v>92</v>
       </c>
-      <c r="C5" s="16">
+      <c r="C5" s="14">
         <f>(NumTestDevelopers * CostTestStandDevelopment) + (NumTestSystems * CostTestStandDeployment) + (TimeToDevelopTestSystemBuy*CostPerDayDeveloper)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="30" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="27" t="s">
         <v>67</v>
       </c>
-      <c r="B6" s="30" t="s">
+      <c r="B6" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="C6" s="16">
+      <c r="C6" s="14">
         <f>TimeToDevelopTestSystem * CostPerDayDeveloper * TimeSpentInMaintenanceBuild_percent / 100 * NumMaintenances_year</f>
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="30" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="27" t="s">
         <v>68</v>
       </c>
-      <c r="B7" s="30" t="s">
+      <c r="B7" s="27" t="s">
         <v>89</v>
       </c>
-      <c r="C7" s="16">
+      <c r="C7" s="14">
         <f>(TimeToDevelopTestSystem * CostPerDayDeveloper * TimeSpentInMaintenanceBuy_percent / 100 * NumMaintenances_year) + (CostSSP * NumTestDevelopers)</f>
         <v>0</v>
       </c>
-      <c r="E7" s="1"/>
-    </row>
-    <row r="8" spans="1:5" s="1" customFormat="1">
-      <c r="A8" s="30" t="s">
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="27" t="s">
         <v>85</v>
       </c>
-      <c r="B8" s="30" t="s">
+      <c r="B8" s="27" t="s">
         <v>87</v>
       </c>
-      <c r="C8" s="16">
+      <c r="C8" s="14">
         <f>CostMaintainTestSystemRecurringBaseBuild * ((1 + IncreaseInMaintenance_percent/100) ^ (LifetimeTestSystem_years-1))</f>
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="1" customFormat="1">
-      <c r="A9" s="30" t="s">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="27" t="s">
         <v>86</v>
       </c>
-      <c r="B9" s="30" t="s">
+      <c r="B9" s="27" t="s">
         <v>88</v>
       </c>
-      <c r="C9" s="16">
+      <c r="C9" s="14">
         <f>CostMaintainTestSystemRecurringBaseBuy * ((1 + IncreaseInMaintenance_percent/100) ^ (LifetimeTestSystem_years-1))</f>
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="30" t="s">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="30" t="s">
+      <c r="B10" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="C10" s="16">
+      <c r="C10" s="14">
         <f>CostPerDayDeveloper * TimeToDevelopTraining_days</f>
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="30" t="s">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="30">
-        <v>0</v>
-      </c>
-      <c r="C11" s="16">
+      <c r="B11" s="27">
+        <v>0</v>
+      </c>
+      <c r="C11" s="14">
         <f>0</f>
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="30" t="s">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="B12" s="30" t="s">
+      <c r="B12" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="C12" s="16">
+      <c r="C12" s="14">
         <f>CostPerDayDeveloper * TimeToReviseTraining_days * NumTrainingRevs_year</f>
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="30" t="s">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="27" t="s">
         <v>70</v>
       </c>
-      <c r="B13" s="30">
-        <v>0</v>
-      </c>
-      <c r="C13" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="30" t="s">
+      <c r="B13" s="27">
+        <v>0</v>
+      </c>
+      <c r="C13" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="B14" s="30" t="s">
+      <c r="B14" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="C14" s="16">
+      <c r="C14" s="14">
         <f>CostPerTrainingBuild</f>
         <v>25000</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
-      <c r="A15" s="30" t="s">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="B15" s="30" t="s">
+      <c r="B15" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="C15" s="16">
+      <c r="C15" s="14">
         <f>CostPerTrainingBuy</f>
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:5" s="1" customFormat="1">
-      <c r="A16" s="30" t="s">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="B16" s="30" t="s">
+      <c r="B16" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="C16" s="16">
+      <c r="C16" s="14">
         <f>CostPerTrainingBuild * NumTrainins_year</f>
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:3" s="1" customFormat="1">
-      <c r="A17" s="30" t="s">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="B17" s="30" t="s">
+      <c r="B17" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="C17" s="16">
+      <c r="C17" s="14">
         <f>CostPerTrainingBuy * NumTrainins_year</f>
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:3" s="1" customFormat="1">
-      <c r="A18" s="30" t="s">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="27" t="s">
         <v>71</v>
       </c>
-      <c r="B18" s="30" t="s">
+      <c r="B18" s="27" t="s">
         <v>93</v>
       </c>
-      <c r="C18" s="16">
+      <c r="C18" s="14">
         <f>CostMaintainTestSystemRecurringBaseBuild*((1-(1+IncreaseInMaintenance_percent/100)^LifetimeTestSystem_years)/(1-(1+IncreaseInMaintenance_percent/100)))</f>
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:3" s="1" customFormat="1">
-      <c r="A19" s="30" t="s">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="27" t="s">
         <v>72</v>
       </c>
-      <c r="B19" s="30" t="s">
+      <c r="B19" s="27" t="s">
         <v>94</v>
       </c>
-      <c r="C19" s="16">
+      <c r="C19" s="14">
         <f>CostMaintainTestSystemRecurringBaseBuy*((1-(1+IncreaseInMaintenance_percent/100)^LifetimeTestSystem_years)/(1-(1+IncreaseInMaintenance_percent/100)))</f>
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:3" s="1" customFormat="1">
-      <c r="A20" s="30" t="s">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="27" t="s">
         <v>73</v>
       </c>
-      <c r="B20" s="30" t="s">
+      <c r="B20" s="27" t="s">
         <v>75</v>
       </c>
-      <c r="C20" s="16">
+      <c r="C20" s="14">
         <f>CostReviseTrainingMaterialBuild * LifetimeTestSystem_years</f>
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:3" s="1" customFormat="1">
-      <c r="A21" s="30" t="s">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="27" t="s">
         <v>74</v>
       </c>
-      <c r="B21" s="30" t="s">
+      <c r="B21" s="27" t="s">
         <v>76</v>
       </c>
-      <c r="C21" s="16">
+      <c r="C21" s="14">
         <f>CostReviseTrainingMaterialBuy * LifetimeTestSystem_years</f>
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:3" s="1" customFormat="1">
-      <c r="A22" s="30" t="s">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="27" t="s">
         <v>63</v>
       </c>
-      <c r="B22" s="30" t="s">
+      <c r="B22" s="27" t="s">
         <v>66</v>
       </c>
-      <c r="C22" s="16">
+      <c r="C22" s="14">
         <f>CostTrainingEmployeesInitialBuild + CostTrainingEmployeesRecurringBuild * LifetimeTestSystem_years</f>
         <v>25000</v>
       </c>
     </row>
-    <row r="23" spans="1:3" s="1" customFormat="1">
-      <c r="A23" s="30" t="s">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="27" t="s">
         <v>64</v>
       </c>
-      <c r="B23" s="30" t="s">
+      <c r="B23" s="27" t="s">
         <v>65</v>
       </c>
-      <c r="C23" s="16">
+      <c r="C23" s="14">
         <f>CostTrainingEmployeesInitialBuy + CostTrainingEmployeesRecurringBuy * LifetimeTestSystem_years</f>
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
-      <c r="A24" s="30" t="s">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="B24" s="30" t="s">
+      <c r="B24" s="27" t="s">
         <v>48</v>
       </c>
-      <c r="C24" s="16">
+      <c r="C24" s="14">
         <f>CostDevelopTestExecutiveBuild + CostDevelopTrainingMaterialBuild + CostTrainingEmployeesInitialBuild</f>
         <v>25000</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
-      <c r="A25" s="30" t="s">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="B25" s="30" t="s">
+      <c r="B25" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="C25" s="16">
+      <c r="C25" s="14">
         <f>CostDevelopTestExecutiveBuy + CostTrainingEmployeesInitialBuy</f>
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
-      <c r="A26" s="30" t="s">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="B26" s="30" t="s">
+      <c r="B26" s="27" t="s">
         <v>95</v>
       </c>
-      <c r="C26" s="16">
+      <c r="C26" s="14">
         <f>CostMaintainTestSystemRecurringBaseBuild + CostReviseTrainingMaterialBuild + CostTrainingEmployeesRecurringBuild</f>
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
-      <c r="A27" s="30" t="s">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="B27" s="30" t="s">
+      <c r="B27" s="27" t="s">
         <v>96</v>
       </c>
-      <c r="C27" s="16">
+      <c r="C27" s="14">
         <f>CostMaintainTestSystemRecurringBaseBuy + CostTrainingEmployeesRecurringBuy</f>
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
-      <c r="A28" s="30" t="s">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="B28" s="30" t="s">
+      <c r="B28" s="27" t="s">
         <v>77</v>
       </c>
-      <c r="C28" s="16">
+      <c r="C28" s="14">
         <f>UpFrontCostBuild + RecurringCostBuild * LifetimeTestSystem_years</f>
         <v>25000</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
-      <c r="A29" s="30" t="s">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="B29" s="30" t="s">
+      <c r="B29" s="27" t="s">
         <v>78</v>
       </c>
-      <c r="C29" s="16">
+      <c r="C29" s="14">
         <f>UpFrontCostBuy + RecurringCostBuy * LifetimeTestSystem_years</f>
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
-      <c r="A30" s="30"/>
-      <c r="B30" s="30"/>
-      <c r="C30" s="16"/>
-    </row>
-    <row r="31" spans="1:3">
-      <c r="A31" s="30" t="s">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="27"/>
+      <c r="B30" s="27"/>
+      <c r="C30" s="14"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="B31" s="30" t="s">
+      <c r="B31" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="C31" s="16">
+      <c r="C31" s="14">
         <f>AvgSalaryDeveloper/NumWorkDays</f>
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
-      <c r="A32" s="30" t="s">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="B32" s="30" t="s">
+      <c r="B32" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="C32" s="16">
+      <c r="C32" s="14">
         <f>AvgSalaryOperator/NumWorkDays</f>
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
-      <c r="A33" s="30" t="s">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="B33" s="30" t="s">
+      <c r="B33" s="27" t="s">
         <v>101</v>
       </c>
-      <c r="C33" s="16">
+      <c r="C33" s="14">
         <f>(IsFeature01*TimeFeature01_days) + (IsFeature02*TimeFeature02_days) + (IsFeature03*TimeFeature03_days) + (IsFeature04*TimeFeature04_days) + (IsFeature05*TimeFeature05_days) + (IsFeature06*TimeFeature06_days) + (IsFeature07*TimeFeature07_days) + (IsFeature08*TimeFeature08_days) + (IsFeature09*(TimeFeature09_days+TimeFeature09PerLanguage_days*(NumDevelopmentLanguages-1))) + (IsFeature10*TimeFeature10_days) + (IsFeature11*TimeFeature11_days) + (IsFeature12*TimeFeature12_days)</f>
         <v>355</v>
       </c>
     </row>
-    <row r="34" spans="1:3" s="1" customFormat="1">
-      <c r="A34" s="30" t="s">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="B34" s="30" t="s">
+      <c r="B34" s="27" t="s">
         <v>97</v>
       </c>
-      <c r="C34" s="16">
+      <c r="C34" s="14">
         <f>(IsFeature01*TimeCustomizeTestStandFeature01_days) + (IsFeature02*TimeCustomizeTestStandFeature02_days) + (IsFeature03*TimeCustomizeTestStandFeature03_days) + (IsFeature04*TimeCustomizeTestStandFeature04_days) + (IsFeature05*TimeCustomizeTestStandFeature05_days) + (IsFeature06*TimeCustomizeTestStandFeature06_days) + (IsFeature07*TimeCustomizeTestStandFeature07_days) + (IsFeature08*TimeCustomizeTestStandFeature08_days) + (IsFeature09*TimeCustomizeTestStandFeature09_days) + (IsFeature10*TimeCustomizeTestStandFeature10_days) + (IsFeature11*TimeCustomizeTestStandFeature11_days) + (IsFeature12*TimeCustomizeTestStandFeature12_days)</f>
         <v>18</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
-      <c r="A35" s="30" t="s">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="B35" s="30" t="s">
+      <c r="B35" s="27" t="s">
         <v>98</v>
       </c>
-      <c r="C35" s="16">
+      <c r="C35" s="14">
         <f>IF(FreqTrainingRevisions_months &lt;&gt; 0, 12/FreqTrainingRevisions_months, 0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
-      <c r="A36" s="30" t="s">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="B36" s="30" t="s">
+      <c r="B36" s="27" t="s">
         <v>100</v>
       </c>
-      <c r="C36" s="16">
+      <c r="C36" s="14">
         <f>IF(FreqTraining_months &lt;&gt; 0, 12/FreqTraining_months, 0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
-      <c r="A37" s="30" t="s">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="B37" s="30" t="s">
+      <c r="B37" s="27" t="s">
         <v>102</v>
       </c>
-      <c r="C37" s="16">
+      <c r="C37" s="14">
         <f>((NumTestDevelopers+1) * CostPerDayDeveloper * DurationDeveloperTraining_hours / 8) + CostTrainingSetupAndPreparation</f>
         <v>25000</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
-      <c r="A38" s="30" t="s">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="B38" s="30" t="s">
+      <c r="B38" s="27" t="s">
         <v>103</v>
       </c>
-      <c r="C38" s="16">
+      <c r="C38" s="14">
         <f>(NumTestDevelopers * CostTestStandTraining) + (NumTestDevelopers * CostPerDayDeveloper * DurationTestStandTraining_hours / 8)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
-      <c r="A39" s="30" t="s">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="B39" s="30" t="s">
+      <c r="B39" s="27" t="s">
         <v>99</v>
       </c>
-      <c r="C39" s="16">
+      <c r="C39" s="14">
         <f>IF(FreqMaintenance_months &lt;&gt; 0, 12 / FreqMaintenance_months, 0)</f>
         <v>0</v>
       </c>

</xml_diff>